<commit_message>
Ajuste UsuarioEventos.tsx tabla inferior editar y eliminar
</commit_message>
<xml_diff>
--- a/Calificaciones_Participantes.xlsx
+++ b/Calificaciones_Participantes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Calificaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCADE80-1238-47B9-A504-2D44C63A3CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002C789-5B0D-4639-8966-3DFDCB381F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40467FD8-C853-4271-8A9D-A393B77FB0D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40467FD8-C853-4271-8A9D-A393B77FB0D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos" sheetId="1" r:id="rId1"/>
-    <sheet name="Menu" sheetId="2" r:id="rId2"/>
+    <sheet name="Datos-Roles" sheetId="1" r:id="rId1"/>
+    <sheet name="Menu-Roles" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="65">
   <si>
     <t>EVENTO</t>
   </si>
@@ -212,13 +212,34 @@
   </si>
   <si>
     <t>Ranking de Calificaciones</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Jurado</t>
+  </si>
+  <si>
+    <t>Gestión de Usuarios</t>
+  </si>
+  <si>
+    <t>Crear Usuario</t>
+  </si>
+  <si>
+    <t>Asignar Eventos a Usuario</t>
+  </si>
+  <si>
+    <t>Asociación Usuarios - Eventos</t>
+  </si>
+  <si>
+    <t>Participante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,8 +247,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,14 +289,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -482,11 +513,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -526,10 +704,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D56BAA-9169-4E6C-810A-795BC49E1BA7}">
   <dimension ref="C3:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -1339,117 +1536,228 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1724DD6-716E-47A2-A4FE-E2FF6D57011C}">
-  <dimension ref="E3:G13"/>
+  <dimension ref="E2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+    </row>
     <row r="4" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="37"/>
+      <c r="F5" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G6" s="47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="35"/>
-      <c r="F5" s="31" t="s">
+    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="35"/>
+      <c r="F7" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G7" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="35"/>
-      <c r="F6" s="41" t="s">
+    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="35"/>
+      <c r="F8" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G8" s="36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="37"/>
-      <c r="F7" s="40" t="s">
+    <row r="9" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="37"/>
+      <c r="F9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G9" s="38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="32" t="s">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F10" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G10" s="34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="35"/>
-      <c r="F9" s="31" t="s">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="35"/>
+      <c r="F11" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G11" s="36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="37"/>
-      <c r="F10" s="40" t="s">
+    <row r="12" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="37"/>
+      <c r="F12" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G12" s="38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="32" t="s">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G13" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="35"/>
-      <c r="F12" s="41" t="s">
+    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="35"/>
+      <c r="F14" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G14" s="36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="37"/>
-      <c r="F13" s="39" t="s">
+    <row r="15" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="37"/>
+      <c r="F15" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G15" s="38" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="17" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
+    </row>
+    <row r="19" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="35"/>
+      <c r="F22" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="37"/>
+      <c r="F23" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="5:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
+    </row>
+    <row r="27" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="51" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E26:G26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualiza EventosPage.tsx con ventana modal valida si tiene categorías asociadas
</commit_message>
<xml_diff>
--- a/Calificaciones_Participantes.xlsx
+++ b/Calificaciones_Participantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Calificaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002C789-5B0D-4639-8966-3DFDCB381F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EE682-7682-4237-9DD4-59D371C5F389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40467FD8-C853-4271-8A9D-A393B77FB0D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{40467FD8-C853-4271-8A9D-A393B77FB0D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos-Roles" sheetId="1" r:id="rId1"/>
@@ -1043,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D56BAA-9169-4E6C-810A-795BC49E1BA7}">
   <dimension ref="C3:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -1538,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1724DD6-716E-47A2-A4FE-E2FF6D57011C}">
   <dimension ref="E2:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>